<commit_message>
added correcter if lineup chages
</commit_message>
<xml_diff>
--- a/lineup.xlsx
+++ b/lineup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="330">
   <si>
     <t xml:space="preserve">sobota 20. 07.</t>
   </si>
@@ -736,6 +736,9 @@
     <t xml:space="preserve">Hypocrisy</t>
   </si>
   <si>
+    <t xml:space="preserve">Peter Tagtgren is my spirit animal &lt;3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Demons &amp; Wizards</t>
   </si>
   <si>
@@ -949,25 +952,64 @@
     <t xml:space="preserve">The Ruins of Beverast</t>
   </si>
   <si>
+    <t xml:space="preserve">atmos black/doom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">počasn ampak dobr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Impaled nazarene</t>
   </si>
   <si>
+    <t xml:space="preserve">definitivno (korpiklaani bojo itk zamujal k bojo pjani)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tiamat</t>
   </si>
   <si>
+    <t xml:space="preserve">gothic/doom neki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preveč rocki (vsaj poznejš) za zaklučt bo dobr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Autopsy night</t>
   </si>
   <si>
+    <t xml:space="preserve">rus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brutal death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">še kr uredu loh blo bolš</t>
+  </si>
+  <si>
     <t xml:space="preserve">Obsolete incarnation</t>
   </si>
   <si>
+    <t xml:space="preserve">propr brutal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Richthammer</t>
   </si>
   <si>
     <t xml:space="preserve">Decaying days</t>
   </si>
   <si>
+    <t xml:space="preserve">melo death/doom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ni slabo bi blo pa lahko bolš</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desdemonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kr klasičn death</t>
   </si>
 </sst>
 </file>
@@ -1153,17 +1195,18 @@
   </sheetPr>
   <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A114" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D151" activeCellId="0" sqref="D151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2613,7 +2656,7 @@
         <v>170</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>141</v>
+        <v>238</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2621,7 +2664,7 @@
         <v>72</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>12</v>
@@ -2630,7 +2673,7 @@
         <v>40</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,53 +2683,53 @@
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>125</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,13 +2737,13 @@
         <v>84</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>203</v>
@@ -2711,7 +2754,7 @@
         <v>87</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>69</v>
@@ -2720,7 +2763,7 @@
         <v>24</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,16 +2771,16 @@
         <v>91</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,16 +2788,16 @@
         <v>95</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>213</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2762,7 +2805,7 @@
         <v>99</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>162</v>
@@ -2771,7 +2814,7 @@
         <v>199</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,13 +2822,13 @@
         <v>103</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>49</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E121" s="0" t="s">
         <v>6</v>
@@ -2801,7 +2844,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>42</v>
@@ -2810,7 +2853,7 @@
         <v>24</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,16 +2861,16 @@
         <v>2</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C125" s="0" t="s">
         <v>118</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,7 +2878,7 @@
         <v>2</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C126" s="0" t="s">
         <v>118</v>
@@ -2844,7 +2887,7 @@
         <v>24</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,16 +2895,16 @@
         <v>2</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2912,7 @@
         <v>2</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>4</v>
@@ -2878,12 +2921,12 @@
         <v>5</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,13 +2939,13 @@
         <v>47</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>216</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>108</v>
@@ -2913,13 +2956,13 @@
         <v>51</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>38</v>
@@ -2930,7 +2973,7 @@
         <v>54</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C134" s="0" t="s">
         <v>12</v>
@@ -2939,7 +2982,7 @@
         <v>24</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,16 +2990,16 @@
         <v>58</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,13 +3007,13 @@
         <v>62</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C136" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E136" s="0" t="s">
         <v>6</v>
@@ -2981,7 +3024,7 @@
         <v>67</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>139</v>
@@ -2998,16 +3041,16 @@
         <v>72</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>162</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,24 +3063,24 @@
         <v>76</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C142" s="0" t="s">
         <v>16</v>
@@ -3051,33 +3094,33 @@
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>233</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C144" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E144" s="0" t="s">
         <v>38</v>
@@ -3088,41 +3131,50 @@
         <v>91</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C145" s="0" t="s">
         <v>69</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E145" s="0" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+    <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B146" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="C146" s="0" t="s">
+      <c r="B146" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C146" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="D146" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B147" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="C147" s="0" t="s">
+      <c r="B147" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C147" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D147" s="0" t="s">
+      <c r="D147" s="1" t="s">
         <v>199</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,10 +3182,16 @@
         <v>103</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C148" s="0" t="s">
         <v>56</v>
+      </c>
+      <c r="D148" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="E148" s="0" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3146,7 +3204,16 @@
         <v>2</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>311</v>
+        <v>317</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="D151" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="E151" s="0" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3154,7 +3221,16 @@
         <v>2</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>312</v>
+        <v>321</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D152" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="E152" s="0" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3162,7 +3238,16 @@
         <v>2</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>313</v>
+        <v>323</v>
+      </c>
+      <c r="C153" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D153" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3170,7 +3255,16 @@
         <v>2</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>314</v>
+        <v>324</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D154" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="E154" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3178,7 +3272,16 @@
         <v>2</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>315</v>
+        <v>327</v>
+      </c>
+      <c r="C155" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="D155" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E155" s="0" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>